<commit_message>
updated contribution spreadsheet for weeks 7 and 8
</commit_message>
<xml_diff>
--- a/team docs/contributions/Contribution.xlsx
+++ b/team docs/contributions/Contribution.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thebk\Documents\QuteeAI-1\team docs\contributions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thebk\Documents\QuteeAI\team docs\contributions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D8D72EA-74B7-49B4-85C2-816447406901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09492873-3406-4C43-B1DC-A85B244ED571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="1476" windowWidth="17280" windowHeight="8964" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -548,8 +548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -744,30 +744,60 @@
       <c r="A7" s="5">
         <v>7</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="B7" s="6">
+        <v>45355</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.16600000000000001</v>
+      </c>
       <c r="J7" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.99600000000000011</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>8</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="B8" s="6">
+        <v>45362</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.16600000000000001</v>
+      </c>
       <c r="J8" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.99600000000000011</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -854,31 +884,31 @@
       </c>
       <c r="C15" s="2">
         <f>SUM(C2:C13)/COUNT(C2:C13)</f>
-        <v>0.17280000000000001</v>
+        <v>0.17085714285714285</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" ref="D15:J15" si="1">SUM(D2:D13)/COUNT(D2:D13)</f>
-        <v>0.17280000000000001</v>
+        <v>0.17085714285714285</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" si="1"/>
-        <v>0.17280000000000001</v>
+        <v>0.17085714285714285</v>
       </c>
       <c r="F15" s="2">
         <f t="shared" si="1"/>
-        <v>0.17280000000000001</v>
+        <v>0.17085714285714285</v>
       </c>
       <c r="G15" s="2">
         <f t="shared" si="1"/>
-        <v>0.15280000000000002</v>
+        <v>0.15657142857142858</v>
       </c>
       <c r="H15" s="2">
         <f t="shared" si="1"/>
-        <v>0.15280000000000002</v>
+        <v>0.15657142857142858</v>
       </c>
       <c r="J15" s="2">
         <f t="shared" si="1"/>
-        <v>0.41533333333333333</v>
+        <v>0.58133333333333337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated contribution spreadsheet for week 10
</commit_message>
<xml_diff>
--- a/team docs/contributions/Contribution.xlsx
+++ b/team docs/contributions/Contribution.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thebk\Documents\QuteeAI\team docs\contributions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09492873-3406-4C43-B1DC-A85B244ED571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBC4437-1193-4548-BBEA-132BE9D0E8EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5760" yWindow="1476" windowWidth="17280" windowHeight="8964" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -548,8 +548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="D3" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -804,15 +804,30 @@
       <c r="A9" s="5">
         <v>9</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="B9" s="6">
+        <v>45369</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.16600000000000001</v>
+      </c>
       <c r="J9" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.99600000000000011</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -884,31 +899,31 @@
       </c>
       <c r="C15" s="2">
         <f>SUM(C2:C13)/COUNT(C2:C13)</f>
-        <v>0.17085714285714285</v>
+        <v>0.17024999999999998</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" ref="D15:J15" si="1">SUM(D2:D13)/COUNT(D2:D13)</f>
-        <v>0.17085714285714285</v>
+        <v>0.17024999999999998</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" si="1"/>
-        <v>0.17085714285714285</v>
+        <v>0.17024999999999998</v>
       </c>
       <c r="F15" s="2">
         <f t="shared" si="1"/>
-        <v>0.17085714285714285</v>
+        <v>0.17024999999999998</v>
       </c>
       <c r="G15" s="2">
         <f t="shared" si="1"/>
-        <v>0.15657142857142858</v>
+        <v>0.15775</v>
       </c>
       <c r="H15" s="2">
         <f t="shared" si="1"/>
-        <v>0.15657142857142858</v>
+        <v>0.15775</v>
       </c>
       <c r="J15" s="2">
         <f t="shared" si="1"/>
-        <v>0.58133333333333337</v>
+        <v>0.66433333333333344</v>
       </c>
     </row>
   </sheetData>

</xml_diff>